<commit_message>
updates scripts for Chapter09
</commit_message>
<xml_diff>
--- a/Chapter10/Chapter10.3.2/position_data.xlsx
+++ b/Chapter10/Chapter10.3.2/position_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason118/PycharmProjects/selenium4.0-automation/Chapter10/Chapter10.3.2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason118/Documents/selenium4.0-automation/Chapter10/Chapter10.3.2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FF8EFB-AA7B-3F47-905F-B8AFD2114C0B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8413B020-8F45-D540-A822-C066F1BD977A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="940" windowWidth="27640" windowHeight="15620" xr2:uid="{ED4AC1EC-C70D-D844-8266-2C2596F1EA1D}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="27640" windowHeight="15620" xr2:uid="{ED4AC1EC-C70D-D844-8266-2C2596F1EA1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Post03052022</t>
+    <t>Post01172023</t>
   </si>
   <si>
-    <t>PostCode03052022</t>
+    <t>PostCode01172023</t>
   </si>
 </sst>
 </file>

</xml_diff>